<commit_message>
Add pagination for books
</commit_message>
<xml_diff>
--- a/ExcelExportService/BorrowedBooks.xlsx
+++ b/ExcelExportService/BorrowedBooks.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BorrowedBooks" sheetId="1" r:id="Re082bb5de7474b74"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BorrowedBooks" sheetId="1" r:id="Rf19d8162367846be"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -47,7 +47,7 @@
         <x:v>False</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>320</x:v>
+        <x:v>460</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -67,7 +67,7 @@
         <x:v>False</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>320</x:v>
+        <x:v>460</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -87,7 +87,7 @@
         <x:v>False</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>320</x:v>
+        <x:v>460</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -107,7 +107,7 @@
         <x:v>False</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>320</x:v>
+        <x:v>460</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -147,7 +147,7 @@
         <x:v>False</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>320</x:v>
+        <x:v>460</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -168,6 +168,126 @@
       </x:c>
       <x:c t="str">
         <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Rendezvous with Rama</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Hasan Çoban</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2025-01-27</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v>False</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>350</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>The Expanse 1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Hasan Çoban</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2025-01-27</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v>False</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Rendezvous with Rama</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>t test1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2025-01-27</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v>False</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>120</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Silo</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qwer qwer</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2025-01-27</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v>False</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Rendezvous with Rama</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>yeni kullanıcı</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2025-01-27</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>14.02.2025 00:00:00</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>False</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>80</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Rendezvous with Rama</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>yeni kullanıcı</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2025-01-27</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>30.01.2025 00:00:00</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>False</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>60</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>